<commit_message>
Atualização do cronograma e criação da apresentação
blalbla
</commit_message>
<xml_diff>
--- a/Docs/2018-04-02 a 2018-04-06 correlatos,RF,RNF,projeto telas e cronograma/Cronograma.xlsx
+++ b/Docs/2018-04-02 a 2018-04-06 correlatos,RF,RNF,projeto telas e cronograma/Cronograma.xlsx
@@ -156,7 +156,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +178,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -209,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -241,12 +247,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,105 +568,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P34"/>
+  <dimension ref="A1:T35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" style="15"/>
     <col min="2" max="2" width="4.28515625" customWidth="1"/>
     <col min="3" max="3" width="77.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
     <col min="5" max="16" width="4" customWidth="1"/>
+    <col min="17" max="20" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E1" s="13" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13" t="s">
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13" t="s">
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-    </row>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E2" s="5" t="s">
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="2" t="s">
+      <c r="C4" s="1"/>
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -674,16 +687,12 @@
       <c r="P4" s="4"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>9</v>
-      </c>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -697,12 +706,12 @@
       <c r="P5" s="4"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>9</v>
@@ -722,79 +731,79 @@
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -814,20 +823,18 @@
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>9</v>
-      </c>
+      <c r="G11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -839,16 +846,18 @@
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="11" t="s">
+      <c r="H12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="12" t="s">
         <v>9</v>
       </c>
       <c r="J12" s="6"/>
@@ -862,16 +871,16 @@
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="11" t="s">
         <v>9</v>
       </c>
       <c r="J13" s="6"/>
@@ -885,19 +894,19 @@
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="11" t="s">
-        <v>9</v>
-      </c>
+      <c r="I14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
@@ -908,20 +917,20 @@
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="14" t="s">
-        <v>9</v>
-      </c>
+      <c r="J15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
@@ -931,10 +940,10 @@
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -942,7 +951,7 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
-      <c r="K16" s="11" t="s">
+      <c r="K16" s="13" t="s">
         <v>9</v>
       </c>
       <c r="L16" s="6"/>
@@ -954,10 +963,10 @@
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="8" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -965,93 +974,93 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="M17" s="14" t="s">
-        <v>9</v>
-      </c>
+      <c r="K17" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="O18" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="P18" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="O19" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="P19" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>9</v>
@@ -1071,15 +1080,15 @@
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7" t="s">
-        <v>9</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
@@ -1094,10 +1103,10 @@
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7" t="s">
@@ -1117,16 +1126,16 @@
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="F24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
@@ -1140,10 +1149,10 @@
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -1163,20 +1172,18 @@
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="G26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
@@ -1188,15 +1195,17 @@
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
+      <c r="H27" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="I27" s="7" t="s">
         <v>9</v>
       </c>
@@ -1211,10 +1220,10 @@
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
@@ -1234,19 +1243,19 @@
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="I29" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" s="7"/>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
@@ -1257,20 +1266,20 @@
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="J30" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K30" s="7"/>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
       <c r="N30" s="7"/>
@@ -1280,10 +1289,10 @@
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -1297,16 +1306,16 @@
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
       <c r="N31" s="7"/>
-      <c r="O31" s="10"/>
+      <c r="O31" s="7"/>
       <c r="P31" s="7"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
@@ -1314,21 +1323,19 @@
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="M32" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="K32" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
       <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
+      <c r="O32" s="10"/>
       <c r="P32" s="7"/>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
-      <c r="C33" s="9" t="s">
-        <v>28</v>
+      <c r="C33" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>11</v>
@@ -1340,46 +1347,71 @@
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O33" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="P33" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="L33" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M33" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="1"/>
+      <c r="C34" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O34" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="P34" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1" t="s">
+      <c r="C35" s="1"/>
+      <c r="D35" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4" t="s">
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="M2:P2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>